<commit_message>
sigue faltando lo mismo
</commit_message>
<xml_diff>
--- a/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
+++ b/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/Cuentas recaudadoras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5A4E8D-69E0-4511-AFF6-71A70F4D5FC2}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45CFDE40-E5C2-4738-B778-0AF71508455E}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="570" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -53,39 +53,129 @@
     <t>ETV M.N</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG ACHUMANI</t>
+  </si>
+  <si>
+    <t>BISA 0022</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG MURILLO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG MAX PAREDES</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISALTO</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG.SATELITE</t>
+  </si>
+  <si>
+    <t>MCSC 6211</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISCRUZ</t>
   </si>
   <si>
     <t>*CERRADA MOMENTANEAMENTE</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA ALEMANA</t>
+  </si>
+  <si>
+    <t>BISA 0049</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA MONTERO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA WARNES</t>
+  </si>
+  <si>
+    <t>MCSC 8183</t>
+  </si>
+  <si>
     <t>ENVIO DE RECAUDACION L-M-V</t>
   </si>
   <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISTAR</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TARIJEÑITA</t>
+  </si>
+  <si>
+    <t>MCSC 1329</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL COCHABAMBA</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG HONDURAS CBBA</t>
+  </si>
+  <si>
+    <t>BISA 0031</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG CALAMA CBBA</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL SUCRE</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA SUCRE 1</t>
+  </si>
+  <si>
+    <t>BISA 0065</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA SUCRE 2</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL POTOSI</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA POTOSI 1</t>
+  </si>
+  <si>
+    <t>BISA 0073</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL ORURO</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA ORURO 1</t>
+  </si>
+  <si>
+    <t>BISA 0057</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL TRINIDAD</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TRINIDAD 1</t>
+  </si>
+  <si>
+    <t>BISA 0090</t>
+  </si>
+  <si>
     <t>DEPOSITO DIARIO</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL PANDO</t>
+  </si>
+  <si>
+    <t>BISA 0111</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL RIBERALTA</t>
+  </si>
+  <si>
+    <t>BISA 0103</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISPAZ</t>
   </si>
   <si>
@@ -185,9 +275,6 @@
     <t>CTA BANCARIA</t>
   </si>
   <si>
-    <t>VALIDACION</t>
-  </si>
-  <si>
     <t>DIRECTO</t>
   </si>
   <si>
@@ -195,6 +282,9 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>EJECUTAR</t>
   </si>
 </sst>
 </file>
@@ -554,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -580,11 +670,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -713,6 +815,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1014,537 +1120,537 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="25"/>
+    <col min="1" max="1" width="27.28515625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>55</v>
+      <c r="F2" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="37">
         <v>101010101</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="41">
         <v>101010102</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="25">
         <v>101020101</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="42">
         <v>101044012</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="38" t="s">
+      <c r="G4" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="41">
+        <v>101010106</v>
+      </c>
+      <c r="D5" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="45">
+        <v>101044012</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="41">
+        <v>101010107</v>
+      </c>
+      <c r="D6" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="45">
+        <v>101044032</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="41">
+        <v>101010109</v>
+      </c>
+      <c r="D7" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="45">
+        <v>101044072</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="41">
+        <v>101010111</v>
+      </c>
+      <c r="D8" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="45">
+        <v>101044022</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="41">
+        <v>101010114</v>
+      </c>
+      <c r="D9" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="45">
+        <v>101044052</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="41">
+        <v>101010117</v>
+      </c>
+      <c r="D10" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="45">
+        <v>101044062</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="41">
+        <v>101010119</v>
+      </c>
+      <c r="D11" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="45">
+        <v>101044042</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="41">
+        <v>101010121</v>
+      </c>
+      <c r="D12" s="25">
+        <v>101020101</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="45">
+        <v>101044082</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="46">
+        <v>101010202</v>
+      </c>
+      <c r="D13" s="47">
+        <v>101020201</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="35">
-        <v>101010106</v>
-      </c>
-      <c r="D5" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="39">
-        <v>101044012</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="35">
-        <v>101010107</v>
-      </c>
-      <c r="D6" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="39">
-        <v>101044032</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="35">
-        <v>101010109</v>
-      </c>
-      <c r="D7" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="39">
-        <v>101044072</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="35">
-        <v>101010111</v>
-      </c>
-      <c r="D8" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="39">
-        <v>101044022</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="35">
-        <v>101010114</v>
-      </c>
-      <c r="D9" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="39">
-        <v>101044052</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="35">
-        <v>101010117</v>
-      </c>
-      <c r="D10" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="39">
-        <v>101044062</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="35">
-        <v>101010119</v>
-      </c>
-      <c r="D11" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="39">
-        <v>101044042</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="35">
-        <v>101010121</v>
-      </c>
-      <c r="D12" s="19">
-        <v>101020101</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="39">
-        <v>101044082</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="40">
-        <v>101010202</v>
-      </c>
-      <c r="D13" s="41">
+      <c r="C14" s="46">
+        <v>101010206</v>
+      </c>
+      <c r="D14" s="48">
         <v>101020201</v>
       </c>
-      <c r="E13" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="40">
-        <v>101010206</v>
-      </c>
-      <c r="D14" s="42">
+      <c r="E14" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="46">
+        <v>101010207</v>
+      </c>
+      <c r="D15" s="48">
         <v>101020201</v>
       </c>
-      <c r="E14" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G14" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="40">
-        <v>101010207</v>
-      </c>
-      <c r="D15" s="42">
+      <c r="E15" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="46">
+        <v>101010209</v>
+      </c>
+      <c r="D16" s="48">
         <v>101020201</v>
       </c>
-      <c r="E15" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G15" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="40">
-        <v>101010209</v>
-      </c>
-      <c r="D16" s="42">
+      <c r="E16" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="46">
+        <v>101010211</v>
+      </c>
+      <c r="D17" s="48">
         <v>101020201</v>
       </c>
-      <c r="E16" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G16" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="40">
-        <v>101010211</v>
-      </c>
-      <c r="D17" s="42">
+      <c r="E17" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="46">
+        <v>101010214</v>
+      </c>
+      <c r="D18" s="48">
         <v>101020201</v>
       </c>
-      <c r="E17" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="40">
-        <v>101010214</v>
-      </c>
-      <c r="D18" s="42">
+      <c r="E18" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="46">
+        <v>101010217</v>
+      </c>
+      <c r="D19" s="48">
         <v>101020201</v>
       </c>
-      <c r="E18" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="40">
-        <v>101010217</v>
-      </c>
-      <c r="D19" s="42">
+      <c r="E19" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="46">
+        <v>101010219</v>
+      </c>
+      <c r="D20" s="48">
         <v>101020201</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="40">
-        <v>101010219</v>
-      </c>
-      <c r="D20" s="42">
+      <c r="E20" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="30">
+        <v>101010221</v>
+      </c>
+      <c r="D21" s="50">
         <v>101020201</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="24">
-        <v>101010221</v>
-      </c>
-      <c r="D21" s="44">
-        <v>101020201</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="39">
-        <v>101052002</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="38" t="s">
-        <v>57</v>
+      <c r="E21" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="45">
+        <v>101052002</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1554,7 +1660,7 @@
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{36543B51-5247-4ED3-ACAE-69DC0A05FC31}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
@@ -1569,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,15 +1689,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="55"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1624,16 +1730,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6">
-        <v>101010203</v>
-      </c>
-      <c r="D4" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>24</v>
+        <v>101010103</v>
+      </c>
+      <c r="D4" s="15">
+        <v>101044012</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1641,16 +1747,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6">
-        <v>101010204</v>
-      </c>
-      <c r="D5" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>24</v>
+        <v>101010104</v>
+      </c>
+      <c r="D5" s="15">
+        <v>101044012</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1658,16 +1764,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6">
-        <v>101010205</v>
-      </c>
-      <c r="D6" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>24</v>
+        <v>101010105</v>
+      </c>
+      <c r="D6" s="15">
+        <v>101044012</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1675,33 +1781,33 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6">
-        <v>101010233</v>
-      </c>
-      <c r="D7" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="17">
-        <v>101010208</v>
-      </c>
-      <c r="D8" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>24</v>
+        <v>101010133</v>
+      </c>
+      <c r="D7" s="15">
+        <v>101041012</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="18">
+        <v>101010108</v>
+      </c>
+      <c r="D8" s="19">
+        <v>101044032</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,16 +1815,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6">
-        <v>101010232</v>
-      </c>
-      <c r="D9" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>24</v>
+        <v>101010132</v>
+      </c>
+      <c r="D9" s="15">
+        <v>101044032</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,16 +1832,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6">
-        <v>101010234</v>
-      </c>
-      <c r="D10" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>24</v>
+        <v>101010134</v>
+      </c>
+      <c r="D10" s="15">
+        <v>101041082</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1743,16 +1849,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6">
-        <v>101010210</v>
-      </c>
-      <c r="D11" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>24</v>
+        <v>101010110</v>
+      </c>
+      <c r="D11" s="15">
+        <v>101041002</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1760,16 +1866,16 @@
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C12" s="6">
-        <v>101010212</v>
-      </c>
-      <c r="D12" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>24</v>
+        <v>101010112</v>
+      </c>
+      <c r="D12" s="15">
+        <v>101044022</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1777,16 +1883,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6">
-        <v>101010213</v>
-      </c>
-      <c r="D13" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>24</v>
+        <v>101010113</v>
+      </c>
+      <c r="D13" s="15">
+        <v>101044022</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1794,16 +1900,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C14" s="6">
-        <v>101010215</v>
-      </c>
-      <c r="D14" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>24</v>
+        <v>101010115</v>
+      </c>
+      <c r="D14" s="15">
+        <v>101044052</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1811,16 +1917,16 @@
         <v>7</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C15" s="6">
-        <v>101010216</v>
-      </c>
-      <c r="D15" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>24</v>
+        <v>101010116</v>
+      </c>
+      <c r="D15" s="15">
+        <v>101044052</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1828,16 +1934,16 @@
         <v>7</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C16" s="6">
-        <v>101010218</v>
-      </c>
-      <c r="D16" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>24</v>
+        <v>101010118</v>
+      </c>
+      <c r="D16" s="15">
+        <v>101044062</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1845,16 +1951,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17" s="6">
-        <v>101010220</v>
-      </c>
-      <c r="D17" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>24</v>
+        <v>101010120</v>
+      </c>
+      <c r="D17" s="15">
+        <v>101044042</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1862,70 +1968,370 @@
         <v>7</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C18" s="6">
-        <v>101010222</v>
-      </c>
-      <c r="D18" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>24</v>
+        <v>101010122</v>
+      </c>
+      <c r="D18" s="15">
+        <v>101044082</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="6">
+        <v>101010136</v>
+      </c>
+      <c r="D19" s="15">
+        <v>101044102</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" s="6">
-        <v>101010236</v>
-      </c>
-      <c r="D19" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="6">
+        <v>101010137</v>
+      </c>
+      <c r="D20" s="15">
+        <v>101044092</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="22">
+        <v>101010201</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="6">
+        <v>101010203</v>
+      </c>
+      <c r="D22" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="6">
+        <v>101010204</v>
+      </c>
+      <c r="D23" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="6">
+        <v>101010205</v>
+      </c>
+      <c r="D24" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="6">
+        <v>101010233</v>
+      </c>
+      <c r="D25" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="18">
+        <v>101010208</v>
+      </c>
+      <c r="D26" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="6">
+        <v>101010232</v>
+      </c>
+      <c r="D27" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="6">
+        <v>101010234</v>
+      </c>
+      <c r="D28" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="6">
+        <v>101010210</v>
+      </c>
+      <c r="D29" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="6">
+        <v>101010212</v>
+      </c>
+      <c r="D30" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="6">
+        <v>101010213</v>
+      </c>
+      <c r="D31" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="6">
+        <v>101010215</v>
+      </c>
+      <c r="D32" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="6">
+        <v>101010216</v>
+      </c>
+      <c r="D33" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="6">
+        <v>101010218</v>
+      </c>
+      <c r="D34" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="6">
+        <v>101010220</v>
+      </c>
+      <c r="D35" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="6">
+        <v>101010222</v>
+      </c>
+      <c r="D36" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="6">
+        <v>101010236</v>
+      </c>
+      <c r="D37" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="6">
         <v>101010237</v>
       </c>
-      <c r="D20" s="18">
-        <v>101052002</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>52</v>
+      <c r="D38" s="24">
+        <v>101052002</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
salto un problema con sapGUI
</commit_message>
<xml_diff>
--- a/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
+++ b/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/Cuentas recaudadoras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B5B7978-DF3D-4E6B-8905-1BC76B74D16B}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_5D9B0ABBCC6F0E33AFA237E5C74618B3C9F96C80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34D734D4-8CC8-4035-9F2B-CF3D12BD5D42}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="89">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -41,6 +41,12 @@
     <t>REAL</t>
   </si>
   <si>
+    <t>CTA BANCARIA</t>
+  </si>
+  <si>
+    <t>EJECUTAR</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA</t>
   </si>
   <si>
@@ -53,6 +59,75 @@
     <t>ETV M.N</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISALTO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISCRUZ</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>CCAJ-SC39/27/202</t>
+  </si>
+  <si>
+    <t>CCAJ-SC39/26/202</t>
+  </si>
+  <si>
+    <t>ENVIO DE RECAUDACION L-M-V</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISTAR</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL COCHABAMBA</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL SUCRE</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL POTOSI</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL ORURO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL TRINIDAD</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISPAZ</t>
+  </si>
+  <si>
+    <t>ETV M.E</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISALTO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISCRUZ</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISTAR</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL COCHABAMBA</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL SUCRE</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL POTOSI</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL ORURO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL TRINIDAD</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AG ACHUMANI</t>
   </si>
   <si>
@@ -65,18 +140,12 @@
     <t>CAJA GENERAL M/N - RECAUDADORA AG MAX PAREDES</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISALTO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AG.SATELITE</t>
   </si>
   <si>
     <t>MCSC 6211</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISCRUZ</t>
-  </si>
-  <si>
     <t>*CERRADA MOMENTANEAMENTE</t>
   </si>
   <si>
@@ -95,21 +164,12 @@
     <t>MCSC 8183</t>
   </si>
   <si>
-    <t>ENVIO DE RECAUDACION L-M-V</t>
-  </si>
-  <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISTAR</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TARIJEÑITA</t>
   </si>
   <si>
     <t>MCSC 1329</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL COCHABAMBA</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AG HONDURAS CBBA</t>
   </si>
   <si>
@@ -119,9 +179,6 @@
     <t>CAJA GENERAL M/N - RECAUDADORA AG CALAMA CBBA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL SUCRE</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA SUCRE 1</t>
   </si>
   <si>
@@ -131,27 +188,18 @@
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA SUCRE 2</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL POTOSI</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA POTOSI 1</t>
   </si>
   <si>
     <t>BISA 0073</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL ORURO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA ORURO 1</t>
   </si>
   <si>
     <t>BISA 0057</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL TRINIDAD</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TRINIDAD 1</t>
   </si>
   <si>
@@ -176,12 +224,6 @@
     <t>CAJA GENERAL M/E - RECAUDADORA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISPAZ</t>
-  </si>
-  <si>
-    <t>ETV M.E</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG ACHUMANI</t>
   </si>
   <si>
@@ -194,15 +236,9 @@
     <t>CAJA GENERAL M/E - RECAUDADORA AG MAX PAREDES</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISALTO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG.SATELITE</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISCRUZ</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA ALEMANA</t>
   </si>
   <si>
@@ -212,45 +248,27 @@
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA WARNES</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISTAR</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA TARIJEÑITA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL COCHABAMBA</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG HONDURAS CBBA</t>
   </si>
   <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG CALAMA CBBA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL SUCRE</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA SUCRE 1</t>
   </si>
   <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA SUCRE 2</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL POTOSI</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA POTOSI 1</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL ORURO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA ORURO 1</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL TRINIDAD</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA TRINIDAD 1</t>
   </si>
   <si>
@@ -270,15 +288,6 @@
   </si>
   <si>
     <t xml:space="preserve">             4) TODOS LOS TRASLADOS SE LOS REALIZA PREVIA VERIFICACION DE INGRESO A BANCO</t>
-  </si>
-  <si>
-    <t>CTA BANCARIA</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>EJECUTAR</t>
   </si>
 </sst>
 </file>
@@ -397,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -656,11 +665,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -805,37 +827,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,10 +924,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1208,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,19 +1234,32 @@
     <col min="1" max="1" width="27.28515625" style="50" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="30"/>
+    <col min="4" max="7" width="11.42578125" style="30" customWidth="1"/>
+    <col min="8" max="9" width="17" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="11.42578125" style="30" customWidth="1"/>
+    <col min="27" max="16384" width="11.42578125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="61"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
@@ -1245,130 +1275,130 @@
       <c r="E2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="69"/>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
-      <c r="AQ2" s="69"/>
-      <c r="AR2" s="69"/>
-      <c r="AS2" s="69"/>
-      <c r="AT2" s="69"/>
-      <c r="AU2" s="69"/>
-      <c r="AV2" s="69"/>
-      <c r="AW2" s="69"/>
-      <c r="AX2" s="69"/>
-      <c r="AY2" s="69"/>
-      <c r="AZ2" s="69"/>
-      <c r="BA2" s="69"/>
-      <c r="BB2" s="69"/>
-      <c r="BC2" s="69"/>
-      <c r="BD2" s="69"/>
+      <c r="F2" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="67"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="58"/>
+      <c r="BB2" s="58"/>
+      <c r="BC2" s="58"/>
+      <c r="BD2" s="58"/>
     </row>
     <row r="3" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" s="35" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="36">
         <v>101010101</v>
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="63"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="69"/>
-      <c r="AB3" s="69"/>
-      <c r="AC3" s="69"/>
-      <c r="AD3" s="69"/>
-      <c r="AE3" s="69"/>
-      <c r="AF3" s="69"/>
-      <c r="AG3" s="69"/>
-      <c r="AH3" s="69"/>
-      <c r="AI3" s="69"/>
-      <c r="AJ3" s="69"/>
-      <c r="AK3" s="69"/>
-      <c r="AL3" s="69"/>
-      <c r="AM3" s="69"/>
-      <c r="AN3" s="69"/>
-      <c r="AO3" s="69"/>
-      <c r="AP3" s="69"/>
-      <c r="AQ3" s="69"/>
-      <c r="AR3" s="69"/>
-      <c r="AS3" s="69"/>
-      <c r="AT3" s="69"/>
-      <c r="AU3" s="69"/>
-      <c r="AV3" s="69"/>
-      <c r="AW3" s="69"/>
-      <c r="AX3" s="69"/>
-      <c r="AY3" s="69"/>
-      <c r="AZ3" s="69"/>
-      <c r="BA3" s="69"/>
-      <c r="BB3" s="69"/>
-      <c r="BC3" s="69"/>
-      <c r="BD3" s="69"/>
-    </row>
-    <row r="4" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
+      <c r="AW3" s="58"/>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="58"/>
+      <c r="BD3" s="58"/>
+    </row>
+    <row r="4" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="40">
         <v>101010102</v>
@@ -1377,70 +1407,70 @@
         <v>101020101</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="41">
         <v>101044012</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="69"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="69"/>
-      <c r="AA4" s="69"/>
-      <c r="AB4" s="69"/>
-      <c r="AC4" s="69"/>
-      <c r="AD4" s="69"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="69"/>
-      <c r="AK4" s="69"/>
-      <c r="AL4" s="69"/>
-      <c r="AM4" s="69"/>
-      <c r="AN4" s="69"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="69"/>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="69"/>
-      <c r="AS4" s="69"/>
-      <c r="AT4" s="69"/>
-      <c r="AU4" s="69"/>
-      <c r="AV4" s="69"/>
-      <c r="AW4" s="69"/>
-      <c r="AX4" s="69"/>
-      <c r="AY4" s="69"/>
-      <c r="AZ4" s="69"/>
-      <c r="BA4" s="69"/>
-      <c r="BB4" s="69"/>
-      <c r="BC4" s="69"/>
-      <c r="BD4" s="69"/>
-    </row>
-    <row r="5" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="58"/>
+      <c r="AD4" s="58"/>
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="58"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="58"/>
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="58"/>
+      <c r="AP4" s="58"/>
+      <c r="AQ4" s="58"/>
+      <c r="AR4" s="58"/>
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="58"/>
+      <c r="AX4" s="58"/>
+      <c r="AY4" s="58"/>
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="58"/>
+    </row>
+    <row r="5" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="40">
         <v>101010106</v>
@@ -1449,70 +1479,70 @@
         <v>101020101</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="43">
         <v>101044012</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="69"/>
-      <c r="Y5" s="69"/>
-      <c r="Z5" s="69"/>
-      <c r="AA5" s="69"/>
-      <c r="AB5" s="69"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="69"/>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="69"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="69"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="69"/>
-      <c r="AK5" s="69"/>
-      <c r="AL5" s="69"/>
-      <c r="AM5" s="69"/>
-      <c r="AN5" s="69"/>
-      <c r="AO5" s="69"/>
-      <c r="AP5" s="69"/>
-      <c r="AQ5" s="69"/>
-      <c r="AR5" s="69"/>
-      <c r="AS5" s="69"/>
-      <c r="AT5" s="69"/>
-      <c r="AU5" s="69"/>
-      <c r="AV5" s="69"/>
-      <c r="AW5" s="69"/>
-      <c r="AX5" s="69"/>
-      <c r="AY5" s="69"/>
-      <c r="AZ5" s="69"/>
-      <c r="BA5" s="69"/>
-      <c r="BB5" s="69"/>
-      <c r="BC5" s="69"/>
-      <c r="BD5" s="69"/>
-    </row>
-    <row r="6" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="58"/>
+      <c r="AD5" s="58"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58"/>
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58"/>
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58"/>
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="58"/>
+    </row>
+    <row r="6" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="40">
         <v>101010107</v>
@@ -1521,70 +1551,74 @@
         <v>101020101</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" s="43">
         <v>101044032</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="69"/>
-      <c r="T6" s="69"/>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
-      <c r="X6" s="69"/>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="69"/>
-      <c r="AA6" s="69"/>
-      <c r="AB6" s="69"/>
-      <c r="AC6" s="69"/>
-      <c r="AD6" s="69"/>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="69"/>
-      <c r="AG6" s="69"/>
-      <c r="AH6" s="69"/>
-      <c r="AI6" s="69"/>
-      <c r="AJ6" s="69"/>
-      <c r="AK6" s="69"/>
-      <c r="AL6" s="69"/>
-      <c r="AM6" s="69"/>
-      <c r="AN6" s="69"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="69"/>
-      <c r="AQ6" s="69"/>
-      <c r="AR6" s="69"/>
-      <c r="AS6" s="69"/>
-      <c r="AT6" s="69"/>
-      <c r="AU6" s="69"/>
-      <c r="AV6" s="69"/>
-      <c r="AW6" s="69"/>
-      <c r="AX6" s="69"/>
-      <c r="AY6" s="69"/>
-      <c r="AZ6" s="69"/>
-      <c r="BA6" s="69"/>
-      <c r="BB6" s="69"/>
-      <c r="BC6" s="69"/>
-      <c r="BD6" s="69"/>
-    </row>
-    <row r="7" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="58"/>
+      <c r="AB6" s="58"/>
+      <c r="AC6" s="58"/>
+      <c r="AD6" s="58"/>
+      <c r="AE6" s="58"/>
+      <c r="AF6" s="58"/>
+      <c r="AG6" s="58"/>
+      <c r="AH6" s="58"/>
+      <c r="AI6" s="58"/>
+      <c r="AJ6" s="58"/>
+      <c r="AK6" s="58"/>
+      <c r="AL6" s="58"/>
+      <c r="AM6" s="58"/>
+      <c r="AN6" s="58"/>
+      <c r="AO6" s="58"/>
+      <c r="AP6" s="58"/>
+      <c r="AQ6" s="58"/>
+      <c r="AR6" s="58"/>
+      <c r="AS6" s="58"/>
+      <c r="AT6" s="58"/>
+      <c r="AU6" s="58"/>
+      <c r="AV6" s="58"/>
+      <c r="AW6" s="58"/>
+      <c r="AX6" s="58"/>
+      <c r="AY6" s="58"/>
+      <c r="AZ6" s="58"/>
+      <c r="BA6" s="58"/>
+      <c r="BB6" s="58"/>
+      <c r="BC6" s="58"/>
+      <c r="BD6" s="58"/>
+    </row>
+    <row r="7" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" s="40">
         <v>101010109</v>
@@ -1593,70 +1627,70 @@
         <v>101020101</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" s="43">
         <v>101044072</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="W7" s="69"/>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="69"/>
-      <c r="AG7" s="69"/>
-      <c r="AH7" s="69"/>
-      <c r="AI7" s="69"/>
-      <c r="AJ7" s="69"/>
-      <c r="AK7" s="69"/>
-      <c r="AL7" s="69"/>
-      <c r="AM7" s="69"/>
-      <c r="AN7" s="69"/>
-      <c r="AO7" s="69"/>
-      <c r="AP7" s="69"/>
-      <c r="AQ7" s="69"/>
-      <c r="AR7" s="69"/>
-      <c r="AS7" s="69"/>
-      <c r="AT7" s="69"/>
-      <c r="AU7" s="69"/>
-      <c r="AV7" s="69"/>
-      <c r="AW7" s="69"/>
-      <c r="AX7" s="69"/>
-      <c r="AY7" s="69"/>
-      <c r="AZ7" s="69"/>
-      <c r="BA7" s="69"/>
-      <c r="BB7" s="69"/>
-      <c r="BC7" s="69"/>
-      <c r="BD7" s="69"/>
-    </row>
-    <row r="8" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="58"/>
+      <c r="AE7" s="58"/>
+      <c r="AF7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="58"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="58"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="58"/>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7" s="58"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7" s="58"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="58"/>
+      <c r="AU7" s="58"/>
+      <c r="AV7" s="58"/>
+      <c r="AW7" s="58"/>
+      <c r="AX7" s="58"/>
+      <c r="AY7" s="58"/>
+      <c r="AZ7" s="58"/>
+      <c r="BA7" s="58"/>
+      <c r="BB7" s="58"/>
+      <c r="BC7" s="58"/>
+      <c r="BD7" s="58"/>
+    </row>
+    <row r="8" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C8" s="40">
         <v>101010111</v>
@@ -1665,70 +1699,70 @@
         <v>101020101</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F8" s="43">
         <v>101044022</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
-      <c r="W8" s="69"/>
-      <c r="X8" s="69"/>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
-      <c r="AA8" s="69"/>
-      <c r="AB8" s="69"/>
-      <c r="AC8" s="69"/>
-      <c r="AD8" s="69"/>
-      <c r="AE8" s="69"/>
-      <c r="AF8" s="69"/>
-      <c r="AG8" s="69"/>
-      <c r="AH8" s="69"/>
-      <c r="AI8" s="69"/>
-      <c r="AJ8" s="69"/>
-      <c r="AK8" s="69"/>
-      <c r="AL8" s="69"/>
-      <c r="AM8" s="69"/>
-      <c r="AN8" s="69"/>
-      <c r="AO8" s="69"/>
-      <c r="AP8" s="69"/>
-      <c r="AQ8" s="69"/>
-      <c r="AR8" s="69"/>
-      <c r="AS8" s="69"/>
-      <c r="AT8" s="69"/>
-      <c r="AU8" s="69"/>
-      <c r="AV8" s="69"/>
-      <c r="AW8" s="69"/>
-      <c r="AX8" s="69"/>
-      <c r="AY8" s="69"/>
-      <c r="AZ8" s="69"/>
-      <c r="BA8" s="69"/>
-      <c r="BB8" s="69"/>
-      <c r="BC8" s="69"/>
-      <c r="BD8" s="69"/>
-    </row>
-    <row r="9" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+      <c r="Z8" s="58"/>
+      <c r="AA8" s="58"/>
+      <c r="AB8" s="58"/>
+      <c r="AC8" s="58"/>
+      <c r="AD8" s="58"/>
+      <c r="AE8" s="58"/>
+      <c r="AF8" s="58"/>
+      <c r="AG8" s="58"/>
+      <c r="AH8" s="58"/>
+      <c r="AI8" s="58"/>
+      <c r="AJ8" s="58"/>
+      <c r="AK8" s="58"/>
+      <c r="AL8" s="58"/>
+      <c r="AM8" s="58"/>
+      <c r="AN8" s="58"/>
+      <c r="AO8" s="58"/>
+      <c r="AP8" s="58"/>
+      <c r="AQ8" s="58"/>
+      <c r="AR8" s="58"/>
+      <c r="AS8" s="58"/>
+      <c r="AT8" s="58"/>
+      <c r="AU8" s="58"/>
+      <c r="AV8" s="58"/>
+      <c r="AW8" s="58"/>
+      <c r="AX8" s="58"/>
+      <c r="AY8" s="58"/>
+      <c r="AZ8" s="58"/>
+      <c r="BA8" s="58"/>
+      <c r="BB8" s="58"/>
+      <c r="BC8" s="58"/>
+      <c r="BD8" s="58"/>
+    </row>
+    <row r="9" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C9" s="40">
         <v>101010114</v>
@@ -1737,70 +1771,70 @@
         <v>101020101</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F9" s="43">
         <v>101044052</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="69"/>
-      <c r="V9" s="69"/>
-      <c r="W9" s="69"/>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="69"/>
-      <c r="AB9" s="69"/>
-      <c r="AC9" s="69"/>
-      <c r="AD9" s="69"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
-      <c r="AH9" s="69"/>
-      <c r="AI9" s="69"/>
-      <c r="AJ9" s="69"/>
-      <c r="AK9" s="69"/>
-      <c r="AL9" s="69"/>
-      <c r="AM9" s="69"/>
-      <c r="AN9" s="69"/>
-      <c r="AO9" s="69"/>
-      <c r="AP9" s="69"/>
-      <c r="AQ9" s="69"/>
-      <c r="AR9" s="69"/>
-      <c r="AS9" s="69"/>
-      <c r="AT9" s="69"/>
-      <c r="AU9" s="69"/>
-      <c r="AV9" s="69"/>
-      <c r="AW9" s="69"/>
-      <c r="AX9" s="69"/>
-      <c r="AY9" s="69"/>
-      <c r="AZ9" s="69"/>
-      <c r="BA9" s="69"/>
-      <c r="BB9" s="69"/>
-      <c r="BC9" s="69"/>
-      <c r="BD9" s="69"/>
-    </row>
-    <row r="10" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="58"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="58"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="58"/>
+      <c r="AD9" s="58"/>
+      <c r="AE9" s="58"/>
+      <c r="AF9" s="58"/>
+      <c r="AG9" s="58"/>
+      <c r="AH9" s="58"/>
+      <c r="AI9" s="58"/>
+      <c r="AJ9" s="58"/>
+      <c r="AK9" s="58"/>
+      <c r="AL9" s="58"/>
+      <c r="AM9" s="58"/>
+      <c r="AN9" s="58"/>
+      <c r="AO9" s="58"/>
+      <c r="AP9" s="58"/>
+      <c r="AQ9" s="58"/>
+      <c r="AR9" s="58"/>
+      <c r="AS9" s="58"/>
+      <c r="AT9" s="58"/>
+      <c r="AU9" s="58"/>
+      <c r="AV9" s="58"/>
+      <c r="AW9" s="58"/>
+      <c r="AX9" s="58"/>
+      <c r="AY9" s="58"/>
+      <c r="AZ9" s="58"/>
+      <c r="BA9" s="58"/>
+      <c r="BB9" s="58"/>
+      <c r="BC9" s="58"/>
+      <c r="BD9" s="58"/>
+    </row>
+    <row r="10" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C10" s="40">
         <v>101010117</v>
@@ -1809,70 +1843,70 @@
         <v>101020101</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10" s="43">
         <v>101044062</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="69"/>
-      <c r="AI10" s="69"/>
-      <c r="AJ10" s="69"/>
-      <c r="AK10" s="69"/>
-      <c r="AL10" s="69"/>
-      <c r="AM10" s="69"/>
-      <c r="AN10" s="69"/>
-      <c r="AO10" s="69"/>
-      <c r="AP10" s="69"/>
-      <c r="AQ10" s="69"/>
-      <c r="AR10" s="69"/>
-      <c r="AS10" s="69"/>
-      <c r="AT10" s="69"/>
-      <c r="AU10" s="69"/>
-      <c r="AV10" s="69"/>
-      <c r="AW10" s="69"/>
-      <c r="AX10" s="69"/>
-      <c r="AY10" s="69"/>
-      <c r="AZ10" s="69"/>
-      <c r="BA10" s="69"/>
-      <c r="BB10" s="69"/>
-      <c r="BC10" s="69"/>
-      <c r="BD10" s="69"/>
-    </row>
-    <row r="11" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="58"/>
+      <c r="Y10" s="58"/>
+      <c r="Z10" s="58"/>
+      <c r="AA10" s="58"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="58"/>
+      <c r="AE10" s="58"/>
+      <c r="AF10" s="58"/>
+      <c r="AG10" s="58"/>
+      <c r="AH10" s="58"/>
+      <c r="AI10" s="58"/>
+      <c r="AJ10" s="58"/>
+      <c r="AK10" s="58"/>
+      <c r="AL10" s="58"/>
+      <c r="AM10" s="58"/>
+      <c r="AN10" s="58"/>
+      <c r="AO10" s="58"/>
+      <c r="AP10" s="58"/>
+      <c r="AQ10" s="58"/>
+      <c r="AR10" s="58"/>
+      <c r="AS10" s="58"/>
+      <c r="AT10" s="58"/>
+      <c r="AU10" s="58"/>
+      <c r="AV10" s="58"/>
+      <c r="AW10" s="58"/>
+      <c r="AX10" s="58"/>
+      <c r="AY10" s="58"/>
+      <c r="AZ10" s="58"/>
+      <c r="BA10" s="58"/>
+      <c r="BB10" s="58"/>
+      <c r="BC10" s="58"/>
+      <c r="BD10" s="58"/>
+    </row>
+    <row r="11" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C11" s="40">
         <v>101010119</v>
@@ -1881,70 +1915,70 @@
         <v>101020101</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" s="43">
         <v>101044042</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="69"/>
-      <c r="S11" s="69"/>
-      <c r="T11" s="69"/>
-      <c r="U11" s="69"/>
-      <c r="V11" s="69"/>
-      <c r="W11" s="69"/>
-      <c r="X11" s="69"/>
-      <c r="Y11" s="69"/>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="69"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
-      <c r="AH11" s="69"/>
-      <c r="AI11" s="69"/>
-      <c r="AJ11" s="69"/>
-      <c r="AK11" s="69"/>
-      <c r="AL11" s="69"/>
-      <c r="AM11" s="69"/>
-      <c r="AN11" s="69"/>
-      <c r="AO11" s="69"/>
-      <c r="AP11" s="69"/>
-      <c r="AQ11" s="69"/>
-      <c r="AR11" s="69"/>
-      <c r="AS11" s="69"/>
-      <c r="AT11" s="69"/>
-      <c r="AU11" s="69"/>
-      <c r="AV11" s="69"/>
-      <c r="AW11" s="69"/>
-      <c r="AX11" s="69"/>
-      <c r="AY11" s="69"/>
-      <c r="AZ11" s="69"/>
-      <c r="BA11" s="69"/>
-      <c r="BB11" s="69"/>
-      <c r="BC11" s="69"/>
-      <c r="BD11" s="69"/>
-    </row>
-    <row r="12" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="58"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="58"/>
+      <c r="AF11" s="58"/>
+      <c r="AG11" s="58"/>
+      <c r="AH11" s="58"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AK11" s="58"/>
+      <c r="AL11" s="58"/>
+      <c r="AM11" s="58"/>
+      <c r="AN11" s="58"/>
+      <c r="AO11" s="58"/>
+      <c r="AP11" s="58"/>
+      <c r="AQ11" s="58"/>
+      <c r="AR11" s="58"/>
+      <c r="AS11" s="58"/>
+      <c r="AT11" s="58"/>
+      <c r="AU11" s="58"/>
+      <c r="AV11" s="58"/>
+      <c r="AW11" s="58"/>
+      <c r="AX11" s="58"/>
+      <c r="AY11" s="58"/>
+      <c r="AZ11" s="58"/>
+      <c r="BA11" s="58"/>
+      <c r="BB11" s="58"/>
+      <c r="BC11" s="58"/>
+      <c r="BD11" s="58"/>
+    </row>
+    <row r="12" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="39" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>42</v>
       </c>
       <c r="C12" s="40">
         <v>101010121</v>
@@ -1953,70 +1987,70 @@
         <v>101020101</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F12" s="43">
         <v>101044082</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
-      <c r="S12" s="69"/>
-      <c r="T12" s="69"/>
-      <c r="U12" s="69"/>
-      <c r="V12" s="69"/>
-      <c r="W12" s="69"/>
-      <c r="X12" s="69"/>
-      <c r="Y12" s="69"/>
-      <c r="Z12" s="69"/>
-      <c r="AA12" s="69"/>
-      <c r="AB12" s="69"/>
-      <c r="AC12" s="69"/>
-      <c r="AD12" s="69"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
-      <c r="AH12" s="69"/>
-      <c r="AI12" s="69"/>
-      <c r="AJ12" s="69"/>
-      <c r="AK12" s="69"/>
-      <c r="AL12" s="69"/>
-      <c r="AM12" s="69"/>
-      <c r="AN12" s="69"/>
-      <c r="AO12" s="69"/>
-      <c r="AP12" s="69"/>
-      <c r="AQ12" s="69"/>
-      <c r="AR12" s="69"/>
-      <c r="AS12" s="69"/>
-      <c r="AT12" s="69"/>
-      <c r="AU12" s="69"/>
-      <c r="AV12" s="69"/>
-      <c r="AW12" s="69"/>
-      <c r="AX12" s="69"/>
-      <c r="AY12" s="69"/>
-      <c r="AZ12" s="69"/>
-      <c r="BA12" s="69"/>
-      <c r="BB12" s="69"/>
-      <c r="BC12" s="69"/>
-      <c r="BD12" s="69"/>
-    </row>
-    <row r="13" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="58"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="58"/>
+      <c r="AF12" s="58"/>
+      <c r="AG12" s="58"/>
+      <c r="AH12" s="58"/>
+      <c r="AI12" s="58"/>
+      <c r="AJ12" s="58"/>
+      <c r="AK12" s="58"/>
+      <c r="AL12" s="58"/>
+      <c r="AM12" s="58"/>
+      <c r="AN12" s="58"/>
+      <c r="AO12" s="58"/>
+      <c r="AP12" s="58"/>
+      <c r="AQ12" s="58"/>
+      <c r="AR12" s="58"/>
+      <c r="AS12" s="58"/>
+      <c r="AT12" s="58"/>
+      <c r="AU12" s="58"/>
+      <c r="AV12" s="58"/>
+      <c r="AW12" s="58"/>
+      <c r="AX12" s="58"/>
+      <c r="AY12" s="58"/>
+      <c r="AZ12" s="58"/>
+      <c r="BA12" s="58"/>
+      <c r="BB12" s="58"/>
+      <c r="BC12" s="58"/>
+      <c r="BD12" s="58"/>
+    </row>
+    <row r="13" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C13" s="44">
         <v>101010202</v>
@@ -2025,70 +2059,70 @@
         <v>101020201</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F13" s="43">
         <v>101052002</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="69"/>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="69"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="69"/>
-      <c r="V13" s="69"/>
-      <c r="W13" s="69"/>
-      <c r="X13" s="69"/>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69"/>
-      <c r="AD13" s="69"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="69"/>
-      <c r="AI13" s="69"/>
-      <c r="AJ13" s="69"/>
-      <c r="AK13" s="69"/>
-      <c r="AL13" s="69"/>
-      <c r="AM13" s="69"/>
-      <c r="AN13" s="69"/>
-      <c r="AO13" s="69"/>
-      <c r="AP13" s="69"/>
-      <c r="AQ13" s="69"/>
-      <c r="AR13" s="69"/>
-      <c r="AS13" s="69"/>
-      <c r="AT13" s="69"/>
-      <c r="AU13" s="69"/>
-      <c r="AV13" s="69"/>
-      <c r="AW13" s="69"/>
-      <c r="AX13" s="69"/>
-      <c r="AY13" s="69"/>
-      <c r="AZ13" s="69"/>
-      <c r="BA13" s="69"/>
-      <c r="BB13" s="69"/>
-      <c r="BC13" s="69"/>
-      <c r="BD13" s="69"/>
-    </row>
-    <row r="14" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58"/>
+      <c r="AD13" s="58"/>
+      <c r="AE13" s="58"/>
+      <c r="AF13" s="58"/>
+      <c r="AG13" s="58"/>
+      <c r="AH13" s="58"/>
+      <c r="AI13" s="58"/>
+      <c r="AJ13" s="58"/>
+      <c r="AK13" s="58"/>
+      <c r="AL13" s="58"/>
+      <c r="AM13" s="58"/>
+      <c r="AN13" s="58"/>
+      <c r="AO13" s="58"/>
+      <c r="AP13" s="58"/>
+      <c r="AQ13" s="58"/>
+      <c r="AR13" s="58"/>
+      <c r="AS13" s="58"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="58"/>
+      <c r="AV13" s="58"/>
+      <c r="AW13" s="58"/>
+      <c r="AX13" s="58"/>
+      <c r="AY13" s="58"/>
+      <c r="AZ13" s="58"/>
+      <c r="BA13" s="58"/>
+      <c r="BB13" s="58"/>
+      <c r="BC13" s="58"/>
+      <c r="BD13" s="58"/>
+    </row>
+    <row r="14" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C14" s="44">
         <v>101010206</v>
@@ -2097,70 +2131,70 @@
         <v>101020201</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F14" s="43">
         <v>101052002</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="69"/>
-      <c r="R14" s="69"/>
-      <c r="S14" s="69"/>
-      <c r="T14" s="69"/>
-      <c r="U14" s="69"/>
-      <c r="V14" s="69"/>
-      <c r="W14" s="69"/>
-      <c r="X14" s="69"/>
-      <c r="Y14" s="69"/>
-      <c r="Z14" s="69"/>
-      <c r="AA14" s="69"/>
-      <c r="AB14" s="69"/>
-      <c r="AC14" s="69"/>
-      <c r="AD14" s="69"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
-      <c r="AH14" s="69"/>
-      <c r="AI14" s="69"/>
-      <c r="AJ14" s="69"/>
-      <c r="AK14" s="69"/>
-      <c r="AL14" s="69"/>
-      <c r="AM14" s="69"/>
-      <c r="AN14" s="69"/>
-      <c r="AO14" s="69"/>
-      <c r="AP14" s="69"/>
-      <c r="AQ14" s="69"/>
-      <c r="AR14" s="69"/>
-      <c r="AS14" s="69"/>
-      <c r="AT14" s="69"/>
-      <c r="AU14" s="69"/>
-      <c r="AV14" s="69"/>
-      <c r="AW14" s="69"/>
-      <c r="AX14" s="69"/>
-      <c r="AY14" s="69"/>
-      <c r="AZ14" s="69"/>
-      <c r="BA14" s="69"/>
-      <c r="BB14" s="69"/>
-      <c r="BC14" s="69"/>
-      <c r="BD14" s="69"/>
-    </row>
-    <row r="15" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+      <c r="AE14" s="58"/>
+      <c r="AF14" s="58"/>
+      <c r="AG14" s="58"/>
+      <c r="AH14" s="58"/>
+      <c r="AI14" s="58"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="58"/>
+      <c r="AL14" s="58"/>
+      <c r="AM14" s="58"/>
+      <c r="AN14" s="58"/>
+      <c r="AO14" s="58"/>
+      <c r="AP14" s="58"/>
+      <c r="AQ14" s="58"/>
+      <c r="AR14" s="58"/>
+      <c r="AS14" s="58"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="58"/>
+      <c r="AV14" s="58"/>
+      <c r="AW14" s="58"/>
+      <c r="AX14" s="58"/>
+      <c r="AY14" s="58"/>
+      <c r="AZ14" s="58"/>
+      <c r="BA14" s="58"/>
+      <c r="BB14" s="58"/>
+      <c r="BC14" s="58"/>
+      <c r="BD14" s="58"/>
+    </row>
+    <row r="15" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C15" s="44">
         <v>101010207</v>
@@ -2169,70 +2203,70 @@
         <v>101020201</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F15" s="43">
         <v>101052002</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="69"/>
-      <c r="S15" s="69"/>
-      <c r="T15" s="69"/>
-      <c r="U15" s="69"/>
-      <c r="V15" s="69"/>
-      <c r="W15" s="69"/>
-      <c r="X15" s="69"/>
-      <c r="Y15" s="69"/>
-      <c r="Z15" s="69"/>
-      <c r="AA15" s="69"/>
-      <c r="AB15" s="69"/>
-      <c r="AC15" s="69"/>
-      <c r="AD15" s="69"/>
-      <c r="AE15" s="69"/>
-      <c r="AF15" s="69"/>
-      <c r="AG15" s="69"/>
-      <c r="AH15" s="69"/>
-      <c r="AI15" s="69"/>
-      <c r="AJ15" s="69"/>
-      <c r="AK15" s="69"/>
-      <c r="AL15" s="69"/>
-      <c r="AM15" s="69"/>
-      <c r="AN15" s="69"/>
-      <c r="AO15" s="69"/>
-      <c r="AP15" s="69"/>
-      <c r="AQ15" s="69"/>
-      <c r="AR15" s="69"/>
-      <c r="AS15" s="69"/>
-      <c r="AT15" s="69"/>
-      <c r="AU15" s="69"/>
-      <c r="AV15" s="69"/>
-      <c r="AW15" s="69"/>
-      <c r="AX15" s="69"/>
-      <c r="AY15" s="69"/>
-      <c r="AZ15" s="69"/>
-      <c r="BA15" s="69"/>
-      <c r="BB15" s="69"/>
-      <c r="BC15" s="69"/>
-      <c r="BD15" s="69"/>
-    </row>
-    <row r="16" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="58"/>
+      <c r="AC15" s="58"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="58"/>
+      <c r="AF15" s="58"/>
+      <c r="AG15" s="58"/>
+      <c r="AH15" s="58"/>
+      <c r="AI15" s="58"/>
+      <c r="AJ15" s="58"/>
+      <c r="AK15" s="58"/>
+      <c r="AL15" s="58"/>
+      <c r="AM15" s="58"/>
+      <c r="AN15" s="58"/>
+      <c r="AO15" s="58"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="58"/>
+      <c r="AR15" s="58"/>
+      <c r="AS15" s="58"/>
+      <c r="AT15" s="58"/>
+      <c r="AU15" s="58"/>
+      <c r="AV15" s="58"/>
+      <c r="AW15" s="58"/>
+      <c r="AX15" s="58"/>
+      <c r="AY15" s="58"/>
+      <c r="AZ15" s="58"/>
+      <c r="BA15" s="58"/>
+      <c r="BB15" s="58"/>
+      <c r="BC15" s="58"/>
+      <c r="BD15" s="58"/>
+    </row>
+    <row r="16" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C16" s="44">
         <v>101010209</v>
@@ -2241,70 +2275,70 @@
         <v>101020201</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F16" s="43">
         <v>101052002</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-      <c r="Q16" s="69"/>
-      <c r="R16" s="69"/>
-      <c r="S16" s="69"/>
-      <c r="T16" s="69"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="69"/>
-      <c r="W16" s="69"/>
-      <c r="X16" s="69"/>
-      <c r="Y16" s="69"/>
-      <c r="Z16" s="69"/>
-      <c r="AA16" s="69"/>
-      <c r="AB16" s="69"/>
-      <c r="AC16" s="69"/>
-      <c r="AD16" s="69"/>
-      <c r="AE16" s="69"/>
-      <c r="AF16" s="69"/>
-      <c r="AG16" s="69"/>
-      <c r="AH16" s="69"/>
-      <c r="AI16" s="69"/>
-      <c r="AJ16" s="69"/>
-      <c r="AK16" s="69"/>
-      <c r="AL16" s="69"/>
-      <c r="AM16" s="69"/>
-      <c r="AN16" s="69"/>
-      <c r="AO16" s="69"/>
-      <c r="AP16" s="69"/>
-      <c r="AQ16" s="69"/>
-      <c r="AR16" s="69"/>
-      <c r="AS16" s="69"/>
-      <c r="AT16" s="69"/>
-      <c r="AU16" s="69"/>
-      <c r="AV16" s="69"/>
-      <c r="AW16" s="69"/>
-      <c r="AX16" s="69"/>
-      <c r="AY16" s="69"/>
-      <c r="AZ16" s="69"/>
-      <c r="BA16" s="69"/>
-      <c r="BB16" s="69"/>
-      <c r="BC16" s="69"/>
-      <c r="BD16" s="69"/>
-    </row>
-    <row r="17" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58"/>
+      <c r="X16" s="58"/>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="58"/>
+      <c r="AC16" s="58"/>
+      <c r="AD16" s="58"/>
+      <c r="AE16" s="58"/>
+      <c r="AF16" s="58"/>
+      <c r="AG16" s="58"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="58"/>
+      <c r="AJ16" s="58"/>
+      <c r="AK16" s="58"/>
+      <c r="AL16" s="58"/>
+      <c r="AM16" s="58"/>
+      <c r="AN16" s="58"/>
+      <c r="AO16" s="58"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="58"/>
+      <c r="AR16" s="58"/>
+      <c r="AS16" s="58"/>
+      <c r="AT16" s="58"/>
+      <c r="AU16" s="58"/>
+      <c r="AV16" s="58"/>
+      <c r="AW16" s="58"/>
+      <c r="AX16" s="58"/>
+      <c r="AY16" s="58"/>
+      <c r="AZ16" s="58"/>
+      <c r="BA16" s="58"/>
+      <c r="BB16" s="58"/>
+      <c r="BC16" s="58"/>
+      <c r="BD16" s="58"/>
+    </row>
+    <row r="17" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C17" s="44">
         <v>101010211</v>
@@ -2313,70 +2347,70 @@
         <v>101020201</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F17" s="43">
         <v>101052002</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="69"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
-      <c r="W17" s="69"/>
-      <c r="X17" s="69"/>
-      <c r="Y17" s="69"/>
-      <c r="Z17" s="69"/>
-      <c r="AA17" s="69"/>
-      <c r="AB17" s="69"/>
-      <c r="AC17" s="69"/>
-      <c r="AD17" s="69"/>
-      <c r="AE17" s="69"/>
-      <c r="AF17" s="69"/>
-      <c r="AG17" s="69"/>
-      <c r="AH17" s="69"/>
-      <c r="AI17" s="69"/>
-      <c r="AJ17" s="69"/>
-      <c r="AK17" s="69"/>
-      <c r="AL17" s="69"/>
-      <c r="AM17" s="69"/>
-      <c r="AN17" s="69"/>
-      <c r="AO17" s="69"/>
-      <c r="AP17" s="69"/>
-      <c r="AQ17" s="69"/>
-      <c r="AR17" s="69"/>
-      <c r="AS17" s="69"/>
-      <c r="AT17" s="69"/>
-      <c r="AU17" s="69"/>
-      <c r="AV17" s="69"/>
-      <c r="AW17" s="69"/>
-      <c r="AX17" s="69"/>
-      <c r="AY17" s="69"/>
-      <c r="AZ17" s="69"/>
-      <c r="BA17" s="69"/>
-      <c r="BB17" s="69"/>
-      <c r="BC17" s="69"/>
-      <c r="BD17" s="69"/>
-    </row>
-    <row r="18" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
+      <c r="W17" s="58"/>
+      <c r="X17" s="58"/>
+      <c r="Y17" s="58"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="58"/>
+      <c r="AC17" s="58"/>
+      <c r="AD17" s="58"/>
+      <c r="AE17" s="58"/>
+      <c r="AF17" s="58"/>
+      <c r="AG17" s="58"/>
+      <c r="AH17" s="58"/>
+      <c r="AI17" s="58"/>
+      <c r="AJ17" s="58"/>
+      <c r="AK17" s="58"/>
+      <c r="AL17" s="58"/>
+      <c r="AM17" s="58"/>
+      <c r="AN17" s="58"/>
+      <c r="AO17" s="58"/>
+      <c r="AP17" s="58"/>
+      <c r="AQ17" s="58"/>
+      <c r="AR17" s="58"/>
+      <c r="AS17" s="58"/>
+      <c r="AT17" s="58"/>
+      <c r="AU17" s="58"/>
+      <c r="AV17" s="58"/>
+      <c r="AW17" s="58"/>
+      <c r="AX17" s="58"/>
+      <c r="AY17" s="58"/>
+      <c r="AZ17" s="58"/>
+      <c r="BA17" s="58"/>
+      <c r="BB17" s="58"/>
+      <c r="BC17" s="58"/>
+      <c r="BD17" s="58"/>
+    </row>
+    <row r="18" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C18" s="44">
         <v>101010214</v>
@@ -2385,70 +2419,70 @@
         <v>101020201</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F18" s="43">
         <v>101052002</v>
       </c>
       <c r="G18" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
-      <c r="Y18" s="69"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="69"/>
-      <c r="AB18" s="69"/>
-      <c r="AC18" s="69"/>
-      <c r="AD18" s="69"/>
-      <c r="AE18" s="69"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="69"/>
-      <c r="AI18" s="69"/>
-      <c r="AJ18" s="69"/>
-      <c r="AK18" s="69"/>
-      <c r="AL18" s="69"/>
-      <c r="AM18" s="69"/>
-      <c r="AN18" s="69"/>
-      <c r="AO18" s="69"/>
-      <c r="AP18" s="69"/>
-      <c r="AQ18" s="69"/>
-      <c r="AR18" s="69"/>
-      <c r="AS18" s="69"/>
-      <c r="AT18" s="69"/>
-      <c r="AU18" s="69"/>
-      <c r="AV18" s="69"/>
-      <c r="AW18" s="69"/>
-      <c r="AX18" s="69"/>
-      <c r="AY18" s="69"/>
-      <c r="AZ18" s="69"/>
-      <c r="BA18" s="69"/>
-      <c r="BB18" s="69"/>
-      <c r="BC18" s="69"/>
-      <c r="BD18" s="69"/>
-    </row>
-    <row r="19" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+      <c r="Y18" s="58"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="58"/>
+      <c r="AF18" s="58"/>
+      <c r="AG18" s="58"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="58"/>
+      <c r="AJ18" s="58"/>
+      <c r="AK18" s="58"/>
+      <c r="AL18" s="58"/>
+      <c r="AM18" s="58"/>
+      <c r="AN18" s="58"/>
+      <c r="AO18" s="58"/>
+      <c r="AP18" s="58"/>
+      <c r="AQ18" s="58"/>
+      <c r="AR18" s="58"/>
+      <c r="AS18" s="58"/>
+      <c r="AT18" s="58"/>
+      <c r="AU18" s="58"/>
+      <c r="AV18" s="58"/>
+      <c r="AW18" s="58"/>
+      <c r="AX18" s="58"/>
+      <c r="AY18" s="58"/>
+      <c r="AZ18" s="58"/>
+      <c r="BA18" s="58"/>
+      <c r="BB18" s="58"/>
+      <c r="BC18" s="58"/>
+      <c r="BD18" s="58"/>
+    </row>
+    <row r="19" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C19" s="44">
         <v>101010217</v>
@@ -2457,70 +2491,70 @@
         <v>101020201</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F19" s="43">
         <v>101052002</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="69"/>
-      <c r="R19" s="69"/>
-      <c r="S19" s="69"/>
-      <c r="T19" s="69"/>
-      <c r="U19" s="69"/>
-      <c r="V19" s="69"/>
-      <c r="W19" s="69"/>
-      <c r="X19" s="69"/>
-      <c r="Y19" s="69"/>
-      <c r="Z19" s="69"/>
-      <c r="AA19" s="69"/>
-      <c r="AB19" s="69"/>
-      <c r="AC19" s="69"/>
-      <c r="AD19" s="69"/>
-      <c r="AE19" s="69"/>
-      <c r="AF19" s="69"/>
-      <c r="AG19" s="69"/>
-      <c r="AH19" s="69"/>
-      <c r="AI19" s="69"/>
-      <c r="AJ19" s="69"/>
-      <c r="AK19" s="69"/>
-      <c r="AL19" s="69"/>
-      <c r="AM19" s="69"/>
-      <c r="AN19" s="69"/>
-      <c r="AO19" s="69"/>
-      <c r="AP19" s="69"/>
-      <c r="AQ19" s="69"/>
-      <c r="AR19" s="69"/>
-      <c r="AS19" s="69"/>
-      <c r="AT19" s="69"/>
-      <c r="AU19" s="69"/>
-      <c r="AV19" s="69"/>
-      <c r="AW19" s="69"/>
-      <c r="AX19" s="69"/>
-      <c r="AY19" s="69"/>
-      <c r="AZ19" s="69"/>
-      <c r="BA19" s="69"/>
-      <c r="BB19" s="69"/>
-      <c r="BC19" s="69"/>
-      <c r="BD19" s="69"/>
-    </row>
-    <row r="20" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="58"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="58"/>
+      <c r="AF19" s="58"/>
+      <c r="AG19" s="58"/>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="58"/>
+      <c r="AJ19" s="58"/>
+      <c r="AK19" s="58"/>
+      <c r="AL19" s="58"/>
+      <c r="AM19" s="58"/>
+      <c r="AN19" s="58"/>
+      <c r="AO19" s="58"/>
+      <c r="AP19" s="58"/>
+      <c r="AQ19" s="58"/>
+      <c r="AR19" s="58"/>
+      <c r="AS19" s="58"/>
+      <c r="AT19" s="58"/>
+      <c r="AU19" s="58"/>
+      <c r="AV19" s="58"/>
+      <c r="AW19" s="58"/>
+      <c r="AX19" s="58"/>
+      <c r="AY19" s="58"/>
+      <c r="AZ19" s="58"/>
+      <c r="BA19" s="58"/>
+      <c r="BB19" s="58"/>
+      <c r="BC19" s="58"/>
+      <c r="BD19" s="58"/>
+    </row>
+    <row r="20" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C20" s="44">
         <v>101010219</v>
@@ -2529,70 +2563,70 @@
         <v>101020201</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F20" s="43">
         <v>101052002</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
-      <c r="X20" s="69"/>
-      <c r="Y20" s="69"/>
-      <c r="Z20" s="69"/>
-      <c r="AA20" s="69"/>
-      <c r="AB20" s="69"/>
-      <c r="AC20" s="69"/>
-      <c r="AD20" s="69"/>
-      <c r="AE20" s="69"/>
-      <c r="AF20" s="69"/>
-      <c r="AG20" s="69"/>
-      <c r="AH20" s="69"/>
-      <c r="AI20" s="69"/>
-      <c r="AJ20" s="69"/>
-      <c r="AK20" s="69"/>
-      <c r="AL20" s="69"/>
-      <c r="AM20" s="69"/>
-      <c r="AN20" s="69"/>
-      <c r="AO20" s="69"/>
-      <c r="AP20" s="69"/>
-      <c r="AQ20" s="69"/>
-      <c r="AR20" s="69"/>
-      <c r="AS20" s="69"/>
-      <c r="AT20" s="69"/>
-      <c r="AU20" s="69"/>
-      <c r="AV20" s="69"/>
-      <c r="AW20" s="69"/>
-      <c r="AX20" s="69"/>
-      <c r="AY20" s="69"/>
-      <c r="AZ20" s="69"/>
-      <c r="BA20" s="69"/>
-      <c r="BB20" s="69"/>
-      <c r="BC20" s="69"/>
-      <c r="BD20" s="69"/>
-    </row>
-    <row r="21" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="58"/>
+      <c r="Y20" s="58"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="58"/>
+      <c r="AC20" s="58"/>
+      <c r="AD20" s="58"/>
+      <c r="AE20" s="58"/>
+      <c r="AF20" s="58"/>
+      <c r="AG20" s="58"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="58"/>
+      <c r="AJ20" s="58"/>
+      <c r="AK20" s="58"/>
+      <c r="AL20" s="58"/>
+      <c r="AM20" s="58"/>
+      <c r="AN20" s="58"/>
+      <c r="AO20" s="58"/>
+      <c r="AP20" s="58"/>
+      <c r="AQ20" s="58"/>
+      <c r="AR20" s="58"/>
+      <c r="AS20" s="58"/>
+      <c r="AT20" s="58"/>
+      <c r="AU20" s="58"/>
+      <c r="AV20" s="58"/>
+      <c r="AW20" s="58"/>
+      <c r="AX20" s="58"/>
+      <c r="AY20" s="58"/>
+      <c r="AZ20" s="58"/>
+      <c r="BA20" s="58"/>
+      <c r="BB20" s="58"/>
+      <c r="BC20" s="58"/>
+      <c r="BD20" s="58"/>
+    </row>
+    <row r="21" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B21" s="47" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="C21" s="29">
         <v>101010221</v>
@@ -2601,63 +2635,63 @@
         <v>101020201</v>
       </c>
       <c r="E21" s="48" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F21" s="43">
         <v>101052002</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="69"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="69"/>
-      <c r="W21" s="69"/>
-      <c r="X21" s="69"/>
-      <c r="Y21" s="69"/>
-      <c r="Z21" s="69"/>
-      <c r="AA21" s="69"/>
-      <c r="AB21" s="69"/>
-      <c r="AC21" s="69"/>
-      <c r="AD21" s="69"/>
-      <c r="AE21" s="69"/>
-      <c r="AF21" s="69"/>
-      <c r="AG21" s="69"/>
-      <c r="AH21" s="69"/>
-      <c r="AI21" s="69"/>
-      <c r="AJ21" s="69"/>
-      <c r="AK21" s="69"/>
-      <c r="AL21" s="69"/>
-      <c r="AM21" s="69"/>
-      <c r="AN21" s="69"/>
-      <c r="AO21" s="69"/>
-      <c r="AP21" s="69"/>
-      <c r="AQ21" s="69"/>
-      <c r="AR21" s="69"/>
-      <c r="AS21" s="69"/>
-      <c r="AT21" s="69"/>
-      <c r="AU21" s="69"/>
-      <c r="AV21" s="69"/>
-      <c r="AW21" s="69"/>
-      <c r="AX21" s="69"/>
-      <c r="AY21" s="69"/>
-      <c r="AZ21" s="69"/>
-      <c r="BA21" s="69"/>
-      <c r="BB21" s="69"/>
-      <c r="BC21" s="69"/>
-      <c r="BD21" s="69"/>
+        <v>12</v>
+      </c>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="58"/>
+      <c r="AF21" s="58"/>
+      <c r="AG21" s="58"/>
+      <c r="AH21" s="58"/>
+      <c r="AI21" s="58"/>
+      <c r="AJ21" s="58"/>
+      <c r="AK21" s="58"/>
+      <c r="AL21" s="58"/>
+      <c r="AM21" s="58"/>
+      <c r="AN21" s="58"/>
+      <c r="AO21" s="58"/>
+      <c r="AP21" s="58"/>
+      <c r="AQ21" s="58"/>
+      <c r="AR21" s="58"/>
+      <c r="AS21" s="58"/>
+      <c r="AT21" s="58"/>
+      <c r="AU21" s="58"/>
+      <c r="AV21" s="58"/>
+      <c r="AW21" s="58"/>
+      <c r="AX21" s="58"/>
+      <c r="AY21" s="58"/>
+      <c r="AZ21" s="58"/>
+      <c r="BA21" s="58"/>
+      <c r="BB21" s="58"/>
+      <c r="BC21" s="58"/>
+      <c r="BD21" s="58"/>
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
@@ -2679,12 +2713,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{36543B51-5247-4ED3-ACAE-69DC0A05FC31}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293"/>
 </worksheet>
 </file>
 
@@ -2704,15 +2738,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2732,7 +2766,7 @@
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9">
         <v>101010101</v>
@@ -2740,15 +2774,15 @@
       <c r="D3" s="10"/>
       <c r="E3" s="51"/>
       <c r="F3" s="56" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6">
         <v>101010103</v>
@@ -2757,18 +2791,18 @@
         <v>101044012</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F4" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6">
         <v>101010104</v>
@@ -2777,18 +2811,18 @@
         <v>101044012</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F5" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6">
         <v>101010105</v>
@@ -2797,18 +2831,18 @@
         <v>101044012</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F6" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6">
         <v>101010133</v>
@@ -2817,18 +2851,18 @@
         <v>101041012</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="F7" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C8" s="17">
         <v>101010108</v>
@@ -2837,18 +2871,18 @@
         <v>101044032</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F8" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C9" s="6">
         <v>101010132</v>
@@ -2857,18 +2891,18 @@
         <v>101044032</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F9" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C10" s="6">
         <v>101010134</v>
@@ -2877,18 +2911,18 @@
         <v>101041082</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6">
         <v>101010110</v>
@@ -2897,18 +2931,18 @@
         <v>101041002</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C12" s="6">
         <v>101010112</v>
@@ -2917,18 +2951,18 @@
         <v>101044022</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F12" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C13" s="6">
         <v>101010113</v>
@@ -2937,18 +2971,18 @@
         <v>101044022</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F13" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C14" s="6">
         <v>101010115</v>
@@ -2957,18 +2991,18 @@
         <v>101044052</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F14" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6">
         <v>101010116</v>
@@ -2977,18 +3011,18 @@
         <v>101044052</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6">
         <v>101010118</v>
@@ -2997,18 +3031,18 @@
         <v>101044062</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F16" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C17" s="6">
         <v>101010120</v>
@@ -3017,18 +3051,18 @@
         <v>101044042</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F17" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C18" s="6">
         <v>101010122</v>
@@ -3037,18 +3071,18 @@
         <v>101044082</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="F18" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C19" s="6">
         <v>101010136</v>
@@ -3057,18 +3091,18 @@
         <v>101044102</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C20" s="6">
         <v>101010137</v>
@@ -3077,16 +3111,16 @@
         <v>101044092</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F20" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C21" s="21">
         <v>101010201</v>
@@ -3097,10 +3131,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C22" s="6">
         <v>101010203</v>
@@ -3109,18 +3143,18 @@
         <v>101052002</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F22" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C23" s="6">
         <v>101010204</v>
@@ -3129,18 +3163,18 @@
         <v>101052002</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F23" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C24" s="6">
         <v>101010205</v>
@@ -3149,18 +3183,18 @@
         <v>101052002</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F24" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C25" s="6">
         <v>101010233</v>
@@ -3169,18 +3203,18 @@
         <v>101052002</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F25" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C26" s="17">
         <v>101010208</v>
@@ -3189,18 +3223,18 @@
         <v>101052002</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F26" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C27" s="6">
         <v>101010232</v>
@@ -3209,18 +3243,18 @@
         <v>101052002</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F27" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C28" s="6">
         <v>101010234</v>
@@ -3229,18 +3263,18 @@
         <v>101052002</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F28" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C29" s="6">
         <v>101010210</v>
@@ -3249,18 +3283,18 @@
         <v>101052002</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F29" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C30" s="6">
         <v>101010212</v>
@@ -3269,18 +3303,18 @@
         <v>101052002</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F30" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C31" s="6">
         <v>101010213</v>
@@ -3289,18 +3323,18 @@
         <v>101052002</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F31" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C32" s="6">
         <v>101010215</v>
@@ -3309,18 +3343,18 @@
         <v>101052002</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F32" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C33" s="6">
         <v>101010216</v>
@@ -3329,18 +3363,18 @@
         <v>101052002</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F33" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C34" s="6">
         <v>101010218</v>
@@ -3349,18 +3383,18 @@
         <v>101052002</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F34" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C35" s="6">
         <v>101010220</v>
@@ -3369,18 +3403,18 @@
         <v>101052002</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F35" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C36" s="6">
         <v>101010222</v>
@@ -3389,18 +3423,18 @@
         <v>101052002</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F36" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C37" s="6">
         <v>101010236</v>
@@ -3409,18 +3443,18 @@
         <v>101052002</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F37" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C38" s="6">
         <v>101010237</v>
@@ -3429,30 +3463,30 @@
         <v>101052002</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F38" s="57" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3472,11 +3506,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bot5 GUI --version 1.00 últimas correcciones
</commit_message>
<xml_diff>
--- a/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
+++ b/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/Cuentas recaudadoras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4F03B46-5EC4-436A-A1AA-44A319EF5CA5}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B490C41-7377-40DE-B189-9BDBAE061EE8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="86">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA MUTUALISTA</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -2674,7 +2671,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,7 +2738,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G4" s="55"/>
     </row>
@@ -2762,7 +2759,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G5" s="55"/>
     </row>
@@ -2783,7 +2780,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G6" s="55"/>
     </row>
@@ -2804,7 +2801,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G7" s="55"/>
     </row>
@@ -2846,7 +2843,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G9" s="55"/>
     </row>
@@ -2867,7 +2864,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G10" s="55"/>
     </row>
@@ -2888,7 +2885,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G11" s="55"/>
     </row>
@@ -2909,7 +2906,7 @@
         <v>29</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G12" s="55"/>
     </row>
@@ -2930,7 +2927,7 @@
         <v>29</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G13" s="55"/>
     </row>
@@ -2951,7 +2948,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G14" s="55"/>
     </row>
@@ -2972,7 +2969,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G15" s="55"/>
     </row>
@@ -2993,7 +2990,7 @@
         <v>37</v>
       </c>
       <c r="F16" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G16" s="55"/>
     </row>
@@ -3014,7 +3011,7 @@
         <v>40</v>
       </c>
       <c r="F17" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G17" s="55"/>
     </row>
@@ -3035,7 +3032,7 @@
         <v>43</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G18" s="55"/>
     </row>
@@ -3056,7 +3053,7 @@
         <v>46</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G19" s="55"/>
     </row>
@@ -3077,7 +3074,7 @@
         <v>48</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G20" s="55"/>
     </row>
@@ -3111,7 +3108,7 @@
         <v>53</v>
       </c>
       <c r="F22" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G22" s="57"/>
     </row>
@@ -3132,7 +3129,7 @@
         <v>53</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3152,7 +3149,7 @@
         <v>53</v>
       </c>
       <c r="F24" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3172,7 +3169,7 @@
         <v>53</v>
       </c>
       <c r="F25" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3192,7 +3189,7 @@
         <v>53</v>
       </c>
       <c r="F26" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3212,7 +3209,7 @@
         <v>53</v>
       </c>
       <c r="F27" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3232,7 +3229,7 @@
         <v>53</v>
       </c>
       <c r="F28" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3252,7 +3249,7 @@
         <v>53</v>
       </c>
       <c r="F29" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3272,7 +3269,7 @@
         <v>53</v>
       </c>
       <c r="F30" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3292,7 +3289,7 @@
         <v>53</v>
       </c>
       <c r="F31" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -3312,7 +3309,7 @@
         <v>53</v>
       </c>
       <c r="F32" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3332,7 +3329,7 @@
         <v>53</v>
       </c>
       <c r="F33" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3352,7 +3349,7 @@
         <v>53</v>
       </c>
       <c r="F34" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3372,7 +3369,7 @@
         <v>53</v>
       </c>
       <c r="F35" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3392,7 +3389,7 @@
         <v>53</v>
       </c>
       <c r="F36" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3412,7 +3409,7 @@
         <v>53</v>
       </c>
       <c r="F37" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3432,7 +3429,7 @@
         <v>53</v>
       </c>
       <c r="F38" s="53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3472,7 +3469,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G20" xr:uid="{6CF02B72-412D-483F-BD39-02D1D4C5A24B}">

</xml_diff>

<commit_message>
Bot5 GUI modificacion de la cantidad de filas de una tabla
</commit_message>
<xml_diff>
--- a/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
+++ b/Cuentas recaudadoras/CUENTAS DE CAJA IVSA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/Cuentas recaudadoras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="8_{E7FEFFEB-5A09-49B6-9D87-359617FDBFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B490C41-7377-40DE-B189-9BDBAE061EE8}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_77C82B5D36F7885256E8FDDD0BA35816BA19BE0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E934D290-257E-44FB-9EA0-95B8ED26E8B3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISTRIBUIDORAS" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="97">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -42,6 +42,12 @@
     <t>REAL</t>
   </si>
   <si>
+    <t>CTA BANCARIA</t>
+  </si>
+  <si>
+    <t>EJECUTAR</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA</t>
   </si>
   <si>
@@ -54,6 +60,99 @@
     <t>ETV M.N</t>
   </si>
   <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>CCAJ-CB11/24/2023</t>
+  </si>
+  <si>
+    <t>CCAJ-TA43/20-21/23</t>
+  </si>
+  <si>
+    <t>CCAJ-CB11/23/2023</t>
+  </si>
+  <si>
+    <t>CCAJ-SC39/42-43/23</t>
+  </si>
+  <si>
+    <t>CCAJ-TR47/19-20/23</t>
+  </si>
+  <si>
+    <t>CCAJ-PT53/16-17/23</t>
+  </si>
+  <si>
+    <t>CCAJ-OR52/17-18/23</t>
+  </si>
+  <si>
+    <t>CCAJ-LP02/36-37/23</t>
+  </si>
+  <si>
+    <t>CCAJ-EA10/35-36/23</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISALTO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISCRUZ</t>
+  </si>
+  <si>
+    <t>ENVIO DE RECAUDACION L-M-V</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISTAR</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL COCHABAMBA</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL SUCRE</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL POTOSI</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL ORURO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL TRINIDAD</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISPAZ</t>
+  </si>
+  <si>
+    <t>ETV M.E</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISALTO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISCRUZ</t>
+  </si>
+  <si>
+    <t>CCAJ-TR47/20/202</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISTAR</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL COCHABAMBA</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL SUCRE</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL POTOSI</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL ORURO</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL TRINIDAD</t>
+  </si>
+  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AG ACHUMANI</t>
   </si>
   <si>
@@ -66,21 +165,18 @@
     <t>CAJA GENERAL M/N - RECAUDADORA AG MAX PAREDES</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISALTO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AG.SATELITE</t>
   </si>
   <si>
     <t>MCSC 6211</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISCRUZ</t>
-  </si>
-  <si>
     <t>*CERRADA MOMENTANEAMENTE</t>
   </si>
   <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA MUTUALISTA</t>
+  </si>
+  <si>
     <t>BISA 0049</t>
   </si>
   <si>
@@ -93,21 +189,12 @@
     <t>MCSC 8183</t>
   </si>
   <si>
-    <t>ENVIO DE RECAUDACION L-M-V</t>
-  </si>
-  <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL DISTAR</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TARIJEÑITA</t>
   </si>
   <si>
     <t>MCSC 1329</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL COCHABAMBA</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AG HONDURAS CBBA</t>
   </si>
   <si>
@@ -117,9 +204,6 @@
     <t>CAJA GENERAL M/N - RECAUDADORA AG CALAMA CBBA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL SUCRE</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA SUCRE 1</t>
   </si>
   <si>
@@ -129,27 +213,18 @@
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA SUCRE 2</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL POTOSI</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA POTOSI 1</t>
   </si>
   <si>
     <t>BISA 0073</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL ORURO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA ORURO 1</t>
   </si>
   <si>
     <t>BISA 0057</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL TRINIDAD</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TRINIDAD 1</t>
   </si>
   <si>
@@ -174,12 +249,6 @@
     <t>CAJA GENERAL M/E - RECAUDADORA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISPAZ</t>
-  </si>
-  <si>
-    <t>ETV M.E</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG ACHUMANI</t>
   </si>
   <si>
@@ -192,13 +261,10 @@
     <t>CAJA GENERAL M/E - RECAUDADORA AG MAX PAREDES</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISALTO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG.SATELITE</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISCRUZ</t>
+    <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA MUTUALISTA</t>
   </si>
   <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA MONTERO</t>
@@ -207,45 +273,27 @@
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA WARNES</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL DISTAR</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA TARIJEÑITA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL COCHABAMBA</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG HONDURAS CBBA</t>
   </si>
   <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AG CALAMA CBBA</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL SUCRE</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA SUCRE 1</t>
   </si>
   <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA SUCRE 2</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL POTOSI</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA POTOSI 1</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL ORURO</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA ORURO 1</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA CENTRAL TRINIDAD</t>
-  </si>
-  <si>
     <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA TRINIDAD 1</t>
   </si>
   <si>
@@ -265,21 +313,6 @@
   </si>
   <si>
     <t xml:space="preserve">             4) TODOS LOS TRASLADOS SE LOS REALIZA PREVIA VERIFICACION DE INGRESO A BANCO</t>
-  </si>
-  <si>
-    <t>CTA BANCARIA</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>EJECUTAR</t>
-  </si>
-  <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA MUTUALISTA</t>
-  </si>
-  <si>
-    <t>CAJA GENERAL M/E - RECAUDADORA AGENCIA MUTUALISTA</t>
   </si>
 </sst>
 </file>
@@ -398,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -644,11 +677,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -799,29 +845,28 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -862,21 +907,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1192,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,19 +1246,29 @@
     <col min="1" max="1" width="27.28515625" style="46" customWidth="1"/>
     <col min="2" max="2" width="47.42578125" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="28"/>
+    <col min="4" max="4" width="11.42578125" style="28" customWidth="1"/>
+    <col min="5" max="7" width="11.42578125" style="28"/>
+    <col min="8" max="8" width="18.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="63" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="62"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29"/>
@@ -1230,12 +1285,12 @@
         <v>5</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="65"/>
+        <v>6</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="67"/>
       <c r="I2" s="54"/>
       <c r="J2" s="54"/>
       <c r="K2" s="54"/>
@@ -1288,23 +1343,22 @@
     <row r="3" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32"/>
       <c r="B3" s="33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="34">
         <v>101010101</v>
       </c>
       <c r="D3" s="35"/>
       <c r="E3" s="36"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="65"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="54"/>
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
       <c r="L3" s="54"/>
       <c r="M3" s="54"/>
       <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
       <c r="P3" s="54"/>
       <c r="Q3" s="54"/>
       <c r="R3" s="54"/>
@@ -1347,12 +1401,12 @@
       <c r="BC3" s="54"/>
       <c r="BD3" s="54"/>
     </row>
-    <row r="4" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="38">
         <v>101010102</v>
@@ -1361,13 +1415,16 @@
         <v>101020101</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F4" s="58">
         <v>101044012</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>20</v>
       </c>
       <c r="I4" s="54"/>
       <c r="J4" s="54"/>
@@ -1418,12 +1475,12 @@
       <c r="BC4" s="54"/>
       <c r="BD4" s="54"/>
     </row>
-    <row r="5" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C5" s="38">
         <v>101010106</v>
@@ -1432,13 +1489,16 @@
         <v>101020101</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="58">
         <v>101044012</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>21</v>
       </c>
       <c r="I5" s="54"/>
       <c r="J5" s="54"/>
@@ -1449,7 +1509,6 @@
       <c r="O5" s="54"/>
       <c r="P5" s="54"/>
       <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
       <c r="S5" s="54"/>
       <c r="T5" s="54"/>
       <c r="U5" s="54"/>
@@ -1489,12 +1548,12 @@
       <c r="BC5" s="54"/>
       <c r="BD5" s="54"/>
     </row>
-    <row r="6" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C6" s="38">
         <v>101010107</v>
@@ -1503,16 +1562,19 @@
         <v>101020101</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" s="58">
         <v>101044032</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>82</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H6"/>
       <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
+      <c r="J6" s="54" t="s">
+        <v>16</v>
+      </c>
       <c r="K6" s="54"/>
       <c r="L6" s="54"/>
       <c r="M6" s="54"/>
@@ -1560,12 +1622,12 @@
       <c r="BC6" s="54"/>
       <c r="BD6" s="54"/>
     </row>
-    <row r="7" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="38">
         <v>101010109</v>
@@ -1574,15 +1636,18 @@
         <v>101020101</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" s="58">
         <v>101044072</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="I7" s="54"/>
+        <v>12</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" s="54" t="s">
+        <v>14</v>
+      </c>
       <c r="J7" s="54"/>
       <c r="K7" s="54"/>
       <c r="L7" s="54"/>
@@ -1631,12 +1696,12 @@
       <c r="BC7" s="54"/>
       <c r="BD7" s="54"/>
     </row>
-    <row r="8" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="38">
         <v>101010111</v>
@@ -1645,21 +1710,25 @@
         <v>101020101</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F8" s="58">
         <v>101044022</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
       </c>
       <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
+      <c r="J8" s="54" t="s">
+        <v>15</v>
+      </c>
       <c r="K8" s="54"/>
       <c r="L8" s="54"/>
       <c r="M8" s="54"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
       <c r="P8" s="54"/>
       <c r="Q8" s="54"/>
       <c r="R8" s="54"/>
@@ -1702,12 +1771,12 @@
       <c r="BC8" s="54"/>
       <c r="BD8" s="54"/>
     </row>
-    <row r="9" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="38">
         <v>101010114</v>
@@ -1716,17 +1785,16 @@
         <v>101020101</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F9" s="58">
         <v>101044052</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="I9" s="54"/>
       <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
       <c r="L9" s="54"/>
       <c r="M9" s="54"/>
       <c r="N9" s="54"/>
@@ -1773,12 +1841,12 @@
       <c r="BC9" s="54"/>
       <c r="BD9" s="54"/>
     </row>
-    <row r="10" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C10" s="38">
         <v>101010117</v>
@@ -1787,15 +1855,17 @@
         <v>101020101</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10" s="58">
         <v>101044062</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="I10" s="54"/>
+        <v>12</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>18</v>
+      </c>
       <c r="J10" s="54"/>
       <c r="K10" s="54"/>
       <c r="L10" s="54"/>
@@ -1844,12 +1914,12 @@
       <c r="BC10" s="54"/>
       <c r="BD10" s="54"/>
     </row>
-    <row r="11" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C11" s="38">
         <v>101010119</v>
@@ -1858,22 +1928,23 @@
         <v>101020101</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" s="58">
         <v>101044042</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>19</v>
       </c>
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
       <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
       <c r="M11" s="54"/>
       <c r="N11" s="54"/>
       <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
       <c r="Q11" s="54"/>
       <c r="R11" s="54"/>
       <c r="S11" s="54"/>
@@ -1915,12 +1986,12 @@
       <c r="BC11" s="54"/>
       <c r="BD11" s="54"/>
     </row>
-    <row r="12" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C12" s="38">
         <v>101010121</v>
@@ -1929,23 +2000,24 @@
         <v>101020101</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F12" s="58">
         <v>101044082</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>17</v>
       </c>
       <c r="I12" s="54"/>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
       <c r="L12" s="54"/>
       <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
       <c r="O12" s="54"/>
       <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
       <c r="R12" s="54"/>
       <c r="S12" s="54"/>
       <c r="T12" s="54"/>
@@ -1986,12 +2058,12 @@
       <c r="BC12" s="54"/>
       <c r="BD12" s="54"/>
     </row>
-    <row r="13" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C13" s="40">
         <v>101010202</v>
@@ -2000,13 +2072,13 @@
         <v>101020201</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F13" s="58">
         <v>101052002</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I13" s="54"/>
       <c r="J13" s="54"/>
@@ -2057,12 +2129,12 @@
       <c r="BC13" s="54"/>
       <c r="BD13" s="54"/>
     </row>
-    <row r="14" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C14" s="40">
         <v>101010206</v>
@@ -2071,13 +2143,13 @@
         <v>101020201</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F14" s="58">
         <v>101052002</v>
       </c>
       <c r="G14" s="39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I14" s="54"/>
       <c r="J14" s="54"/>
@@ -2128,12 +2200,12 @@
       <c r="BC14" s="54"/>
       <c r="BD14" s="54"/>
     </row>
-    <row r="15" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C15" s="40">
         <v>101010207</v>
@@ -2142,16 +2214,19 @@
         <v>101020201</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F15" s="58">
         <v>101052002</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>82</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H15"/>
       <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
+      <c r="J15" s="54" t="s">
+        <v>16</v>
+      </c>
       <c r="K15" s="54"/>
       <c r="L15" s="54"/>
       <c r="M15" s="54"/>
@@ -2199,12 +2274,12 @@
       <c r="BC15" s="54"/>
       <c r="BD15" s="54"/>
     </row>
-    <row r="16" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C16" s="40">
         <v>101010209</v>
@@ -2213,13 +2288,13 @@
         <v>101020201</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F16" s="58">
         <v>101052002</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I16" s="54"/>
       <c r="J16" s="54"/>
@@ -2270,12 +2345,12 @@
       <c r="BC16" s="54"/>
       <c r="BD16" s="54"/>
     </row>
-    <row r="17" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C17" s="40">
         <v>101010211</v>
@@ -2284,15 +2359,20 @@
         <v>101020201</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F17" s="58">
         <v>101052002</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="54"/>
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>15</v>
+      </c>
       <c r="J17" s="54"/>
       <c r="K17" s="54"/>
       <c r="L17" s="54"/>
@@ -2341,12 +2421,12 @@
       <c r="BC17" s="54"/>
       <c r="BD17" s="54"/>
     </row>
-    <row r="18" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C18" s="40">
         <v>101010214</v>
@@ -2355,13 +2435,13 @@
         <v>101020201</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F18" s="58">
         <v>101052002</v>
       </c>
       <c r="G18" s="39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
@@ -2412,12 +2492,12 @@
       <c r="BC18" s="54"/>
       <c r="BD18" s="54"/>
     </row>
-    <row r="19" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C19" s="40">
         <v>101010217</v>
@@ -2426,13 +2506,13 @@
         <v>101020201</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F19" s="58">
         <v>101052002</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I19" s="54"/>
       <c r="J19" s="54"/>
@@ -2483,12 +2563,12 @@
       <c r="BC19" s="54"/>
       <c r="BD19" s="54"/>
     </row>
-    <row r="20" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C20" s="40">
         <v>101010219</v>
@@ -2497,13 +2577,13 @@
         <v>101020201</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F20" s="58">
         <v>101052002</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I20" s="54"/>
       <c r="J20" s="54"/>
@@ -2554,12 +2634,12 @@
       <c r="BC20" s="54"/>
       <c r="BD20" s="54"/>
     </row>
-    <row r="21" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C21" s="27">
         <v>101010221</v>
@@ -2568,17 +2648,19 @@
         <v>101020201</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F21" s="58">
         <v>101052002</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>36</v>
       </c>
       <c r="I21" s="54"/>
       <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
       <c r="L21" s="54"/>
       <c r="M21" s="54"/>
       <c r="N21" s="54"/>
@@ -2637,32 +2719,20 @@
     <mergeCell ref="H2:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:G21">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",G4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",G4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{36543B51-5247-4ED3-ACAE-69DC0A05FC31}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50EF1DB0-88D6-4C93-AB37-ABB00C223944}">
-          <x14:formula1>
-            <xm:f>Hoja1!$A$1:$A$26</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4:F21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293"/>
 </worksheet>
 </file>
 
@@ -2670,8 +2740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,15 +2752,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="69" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="68"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2710,7 +2780,7 @@
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9">
         <v>101010101</v>
@@ -2718,15 +2788,15 @@
       <c r="D3" s="10"/>
       <c r="E3" s="47"/>
       <c r="F3" s="52" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C4" s="6">
         <v>101010103</v>
@@ -2735,19 +2805,19 @@
         <v>101044012</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G4" s="55"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C5" s="6">
         <v>101010104</v>
@@ -2756,19 +2826,19 @@
         <v>101044012</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G5" s="55"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6">
         <v>101010105</v>
@@ -2777,19 +2847,19 @@
         <v>101044012</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G6" s="55"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C7" s="6">
         <v>101010133</v>
@@ -2798,19 +2868,19 @@
         <v>101041012</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G7" s="55"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C8" s="17">
         <v>101010108</v>
@@ -2819,19 +2889,19 @@
         <v>101044032</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C9" s="6">
         <v>101010132</v>
@@ -2840,19 +2910,19 @@
         <v>101044032</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G9" s="55"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6">
         <v>101010134</v>
@@ -2861,19 +2931,19 @@
         <v>101041082</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6">
         <v>101010110</v>
@@ -2882,19 +2952,19 @@
         <v>101041002</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G11" s="55"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="C12" s="6">
         <v>101010112</v>
@@ -2903,19 +2973,19 @@
         <v>101044022</v>
       </c>
       <c r="E12" s="48" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G12" s="55"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6">
         <v>101010113</v>
@@ -2924,19 +2994,19 @@
         <v>101044022</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G13" s="55"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C14" s="6">
         <v>101010115</v>
@@ -2945,19 +3015,19 @@
         <v>101044052</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G14" s="55"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C15" s="6">
         <v>101010116</v>
@@ -2966,19 +3036,19 @@
         <v>101044052</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G15" s="55"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C16" s="6">
         <v>101010118</v>
@@ -2987,19 +3057,19 @@
         <v>101044062</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="F16" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G16" s="55"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C17" s="6">
         <v>101010120</v>
@@ -3008,19 +3078,19 @@
         <v>101044042</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F17" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G17" s="55"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C18" s="6">
         <v>101010122</v>
@@ -3029,19 +3099,19 @@
         <v>101044082</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G18" s="55"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C19" s="6">
         <v>101010136</v>
@@ -3050,19 +3120,19 @@
         <v>101044102</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="G19" s="55"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C20" s="6">
         <v>101010137</v>
@@ -3071,17 +3141,17 @@
         <v>101044092</v>
       </c>
       <c r="E20" s="48" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="19" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C21" s="20">
         <v>101010201</v>
@@ -3093,10 +3163,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C22" s="6">
         <v>101010203</v>
@@ -3105,19 +3175,19 @@
         <v>101052002</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F22" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="G22" s="57"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C23" s="6">
         <v>101010204</v>
@@ -3126,18 +3196,18 @@
         <v>101052002</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C24" s="6">
         <v>101010205</v>
@@ -3146,18 +3216,18 @@
         <v>101052002</v>
       </c>
       <c r="E24" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F24" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C25" s="6">
         <v>101010233</v>
@@ -3166,18 +3236,18 @@
         <v>101052002</v>
       </c>
       <c r="E25" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F25" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C26" s="17">
         <v>101010208</v>
@@ -3186,18 +3256,18 @@
         <v>101052002</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F26" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C27" s="6">
         <v>101010232</v>
@@ -3206,18 +3276,18 @@
         <v>101052002</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F27" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C28" s="6">
         <v>101010234</v>
@@ -3226,18 +3296,18 @@
         <v>101052002</v>
       </c>
       <c r="E28" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F28" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C29" s="6">
         <v>101010210</v>
@@ -3246,18 +3316,18 @@
         <v>101052002</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F29" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C30" s="6">
         <v>101010212</v>
@@ -3266,18 +3336,18 @@
         <v>101052002</v>
       </c>
       <c r="E30" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F30" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C31" s="6">
         <v>101010213</v>
@@ -3286,18 +3356,18 @@
         <v>101052002</v>
       </c>
       <c r="E31" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F31" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C32" s="6">
         <v>101010215</v>
@@ -3306,18 +3376,18 @@
         <v>101052002</v>
       </c>
       <c r="E32" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F32" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C33" s="6">
         <v>101010216</v>
@@ -3326,18 +3396,18 @@
         <v>101052002</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F33" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C34" s="6">
         <v>101010218</v>
@@ -3346,18 +3416,18 @@
         <v>101052002</v>
       </c>
       <c r="E34" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F34" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C35" s="6">
         <v>101010220</v>
@@ -3366,18 +3436,18 @@
         <v>101052002</v>
       </c>
       <c r="E35" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F35" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C36" s="6">
         <v>101010222</v>
@@ -3386,18 +3456,18 @@
         <v>101052002</v>
       </c>
       <c r="E36" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F36" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C37" s="6">
         <v>101010236</v>
@@ -3406,18 +3476,18 @@
         <v>101052002</v>
       </c>
       <c r="E37" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F37" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C38" s="6">
         <v>101010237</v>
@@ -3426,30 +3496,30 @@
         <v>101052002</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="F38" s="53" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3458,43 +3528,31 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F38">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{4DDA8D3B-06EF-40B5-B0B2-CBEB1310B5C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F20 F22:F38" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G20" xr:uid="{6CF02B72-412D-483F-BD39-02D1D4C5A24B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G20" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"101044032,101044042,101044012,101044082,101044052,101044022,101044062,101044102,101041002,101041012,101041082,101044092,101044072,101044002"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DE757339-8787-490F-892F-3451C25EEE25}">
-          <x14:formula1>
-            <xm:f>Hoja1!$A$1:$A$26</xm:f>
-          </x14:formula1>
-          <xm:sqref>D22:D38 D4:D20</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDB91D8-B6A7-47AC-8AE5-E5652C735329}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3635,7 +3693,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25" xr:uid="{9F1E8086-2992-4260-B7D0-122C2D5EBCD7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"101052002,101044002,101044012,101044022,101044032,101044042,101044052,101044062,101044072,101044082,101051002,101041032,101041022,101041012,101041002,101043002,101042022,101051012,101041042,101041052,101041082,101043042,101042012,101045012,101044092"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>